<commit_message>
work deep 15 2023-03-15
</commit_message>
<xml_diff>
--- a/015 VBA Programming/05-05-the-unique-function.xlsx
+++ b/015 VBA Programming/05-05-the-unique-function.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web learning\015 VBA Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{451B70EE-10F1-4A64-B632-CBC9E24C8F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E9C0F85-FDFF-4177-8ED0-BEEA0B99F89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D77D9FF2-12C2-4195-A208-879813459C64}"/>
   </bookViews>
@@ -16,10 +16,10 @@
     <sheet name="The UNIQUE Function" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'The UNIQUE Function'!$A$4:$D$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'The UNIQUE Function'!$B$4:$B$29</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">'The UNIQUE Function'!$F$11</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -105,32 +105,13 @@
   </si>
   <si>
     <t>Matthew</t>
-  </si>
-  <si>
-    <t>Ali</t>
-  </si>
-  <si>
-    <t>Niloofar</t>
-  </si>
-  <si>
-    <t>Shareza</t>
-  </si>
-  <si>
-    <t>Esfahan</t>
-  </si>
-  <si>
-    <t>Shiraz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,12 +132,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -172,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -185,7 +160,18 @@
         <color theme="4" tint="0.39997558519241921"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -194,65 +180,29 @@
       <right style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/mm/dd"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -268,22 +218,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F31BC8A-B98E-4612-8046-DAAC8295AB69}" name="Table1" displayName="Table1" ref="A4:D38" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="2">
-  <autoFilter ref="A4:D38" xr:uid="{03AEB1D8-2594-4508-B452-06704199F5C9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D29">
-    <sortCondition ref="B4:B29"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C6460FA2-B610-47B7-AF88-C3A896855686}" name="Date" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{BE1B4337-76F1-4868-8E32-D3F07E0594FB}" name="Sales Rep"/>
-    <tableColumn id="3" xr3:uid="{E61902CE-CD92-4F56-BB85-C5DFBF888EF6}" name="Region"/>
-    <tableColumn id="4" xr3:uid="{EB99560F-0FFF-43F4-AAED-6E762832DABD}" name="Sales"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -583,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03AEB1D8-2594-4508-B452-06704199F5C9}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -596,7 +530,7 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="10.75" customWidth="1"/>
     <col min="6" max="6" width="11.375" customWidth="1"/>
-    <col min="7" max="7" width="59.875" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
     <col min="8" max="8" width="11.25" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
@@ -607,16 +541,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F4" t="s">
@@ -625,133 +559,123 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43863</v>
+        <v>44137</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>6879</v>
-      </c>
-      <c r="F5" t="str" cm="1">
-        <f t="array" ref="F5:F12">_xlfn.UNIQUE(Table1[Sales Rep])</f>
-        <v>Adam</v>
-      </c>
-      <c r="G5" t="str" cm="1">
-        <f t="array" ref="G5">_xlfn.TEXTJOIN(",",TRUE,(_xlfn.UNIQUE(IF(Table1[Sales Rep]=F5,Table1[Region],""),FALSE,FALSE)))</f>
-        <v>Europe,Asia</v>
-      </c>
-      <c r="H5" s="4" cm="1">
-        <f t="array" ref="H5">SUM(IF(Table1[Sales Rep]=F5,Table1[Sales],""))</f>
-        <v>30046</v>
+        <v>7139</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44106</v>
+        <v>44471</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>9283</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Ben</v>
+        <v>6745</v>
+      </c>
+      <c r="F6" t="str" cm="1">
+        <f t="array" ref="F6:F31">_xlfn.UNIQUE(B4:B29,TRUE,FALSE)</f>
+        <v>Sales Rep</v>
       </c>
       <c r="G6" t="str" cm="1">
-        <f t="array" ref="G6">_xlfn.TEXTJOIN(",",TRUE,(_xlfn.UNIQUE(IF(Table1[Sales Rep]=F6,Table1[Region],""),FALSE,FALSE)))</f>
-        <v>North America,Asia</v>
-      </c>
-      <c r="H6" s="4" cm="1">
-        <f t="array" ref="H6">SUM(IF(Table1[Sales Rep]=F6,Table1[Sales],""))</f>
-        <v>46926</v>
+        <f t="array" ref="G6:G31">_xlfn.UNIQUE(B4:B29,TRUE,TRUE)</f>
+        <v>Sales Rep</v>
+      </c>
+      <c r="H6" t="str" cm="1">
+        <f t="array" ref="H6:H7">_xlfn.UNIQUE(B4:B29,FALSE,TRUE)</f>
+        <v>Sales Rep</v>
+      </c>
+      <c r="I6" t="str" cm="1">
+        <f t="array" ref="I6:I12">_xlfn.UNIQUE(B4:B29,FALSE,FALSE)</f>
+        <v>Sales Rep</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44137</v>
+        <v>43863</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>7139</v>
+        <v>6879</v>
       </c>
       <c r="F7" t="str">
-        <v>Deb</v>
-      </c>
-      <c r="G7" t="str" cm="1">
-        <f t="array" ref="G7">_xlfn.TEXTJOIN(",",TRUE,(_xlfn.UNIQUE(IF(Table1[Sales Rep]=F7,Table1[Region],""),FALSE,FALSE)))</f>
-        <v>Europe,North America</v>
-      </c>
-      <c r="H7" s="4" cm="1">
-        <f t="array" ref="H7">SUM(IF(Table1[Sales Rep]=F7,Table1[Sales],""))</f>
-        <v>33660</v>
+        <v>Adam</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Adam</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Matthew</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Adam</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44471</v>
+        <v>44106</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>6745</v>
+        <v>9283</v>
       </c>
       <c r="F8" t="str">
-        <v>Matthew</v>
-      </c>
-      <c r="G8" t="str" cm="1">
-        <f t="array" ref="G8">_xlfn.TEXTJOIN(",",TRUE,(_xlfn.UNIQUE(IF(Table1[Sales Rep]=F8,Table1[Region],""),FALSE,FALSE)))</f>
-        <v>Asia</v>
-      </c>
-      <c r="H8" s="4" cm="1">
-        <f t="array" ref="H8">SUM(IF(Table1[Sales Rep]=F8,Table1[Sales],""))</f>
-        <v>5000</v>
+        <v>Adam</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Adam</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Ben</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43832</v>
+        <v>44167</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9">
-        <v>8199</v>
+        <v>6978</v>
       </c>
       <c r="F9" t="str">
-        <v>Susie</v>
-      </c>
-      <c r="G9" t="str" cm="1">
-        <f t="array" ref="G9">_xlfn.TEXTJOIN(",",TRUE,(_xlfn.UNIQUE(IF(Table1[Sales Rep]=F9,Table1[Region],""),FALSE,FALSE)))</f>
-        <v>North America,Asia,Europe</v>
-      </c>
-      <c r="H9" s="4" cm="1">
-        <f t="array" ref="H9">SUM(IF(Table1[Sales Rep]=F9,Table1[Sales],""))</f>
-        <v>36886</v>
+        <v>Adam</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Adam</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Deb</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44167</v>
+        <v>44229</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -760,23 +684,21 @@
         <v>11</v>
       </c>
       <c r="D10">
-        <v>6978</v>
+        <v>9050</v>
       </c>
       <c r="F10" t="str">
-        <v>Tom</v>
-      </c>
-      <c r="G10" t="str" cm="1">
-        <f t="array" ref="G10">_xlfn.TEXTJOIN(",",TRUE,(_xlfn.UNIQUE(IF(Table1[Sales Rep]=F10,Table1[Region],""),FALSE,FALSE)))</f>
-        <v>Asia,Europe,North America</v>
-      </c>
-      <c r="H10" s="4" cm="1">
-        <f t="array" ref="H10">SUM(IF(Table1[Sales Rep]=F10,Table1[Sales],""))</f>
-        <v>39215</v>
+        <v>Adam</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Adam</v>
+      </c>
+      <c r="I10" t="str">
+        <v>Matthew</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44198</v>
+        <v>43832</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -785,43 +707,39 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>7631</v>
+        <v>8199</v>
       </c>
       <c r="F11" t="str">
-        <v>Ali</v>
-      </c>
-      <c r="G11" t="str" cm="1">
-        <f t="array" ref="G11">_xlfn.TEXTJOIN(",",TRUE,(_xlfn.UNIQUE(IF(Table1[Sales Rep]=F11,Table1[Region],""),FALSE,FALSE)))</f>
-        <v>Shareza,Esfahan,Shiraz,North America,Asia</v>
-      </c>
-      <c r="H11" s="4" cm="1">
-        <f t="array" ref="H11">SUM(IF(Table1[Sales Rep]=F11,Table1[Sales],""))</f>
-        <v>47478</v>
+        <v>Ben</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Ben</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Susie</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44229</v>
+        <v>44198</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>9050</v>
+        <v>7631</v>
       </c>
       <c r="F12" t="str">
-        <v>Niloofar</v>
-      </c>
-      <c r="G12" t="str" cm="1">
-        <f t="array" ref="G12">_xlfn.TEXTJOIN(",",TRUE,(_xlfn.UNIQUE(IF(Table1[Sales Rep]=F12,Table1[Region],""),FALSE,FALSE)))</f>
-        <v>Esfahan,Shareza</v>
-      </c>
-      <c r="H12" s="4" cm="1">
-        <f t="array" ref="H12">SUM(IF(Table1[Sales Rep]=F12,Table1[Sales],""))</f>
-        <v>22214</v>
+        <v>Ben</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Ben</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Tom</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -837,6 +755,12 @@
       <c r="D13">
         <v>6827</v>
       </c>
+      <c r="F13" t="str">
+        <v>Ben</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Ben</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -851,6 +775,12 @@
       <c r="D14">
         <v>8241</v>
       </c>
+      <c r="F14" t="str">
+        <v>Ben</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Ben</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -865,25 +795,37 @@
       <c r="D15">
         <v>8562</v>
       </c>
+      <c r="F15" t="str">
+        <v>Ben</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Ben</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>44045</v>
+        <v>44257</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>9454</v>
+        <v>8278</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Ben</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Ben</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>44257</v>
+        <v>44410</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -892,25 +834,35 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>8278</v>
-      </c>
-      <c r="F17" s="1"/>
+        <v>7366</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <v>Deb</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Deb</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>44410</v>
+        <v>44045</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18">
-        <v>7366</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>9454</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <v>Deb</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Deb</v>
+      </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -926,28 +878,38 @@
       <c r="D19">
         <v>5000</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="str">
+        <v>Deb</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Deb</v>
+      </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>43923</v>
+        <v>44076</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>9715</v>
-      </c>
-      <c r="F20" s="1"/>
+        <v>5279</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <v>Deb</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Deb</v>
+      </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>44076</v>
+        <v>44318</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -956,57 +918,77 @@
         <v>11</v>
       </c>
       <c r="D21">
-        <v>5279</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>7524</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <v>Matthew</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Matthew</v>
+      </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>44288</v>
+        <v>44532</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>8351</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>6017</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <v>Susie</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Susie</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>44318</v>
+        <v>44288</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23">
-        <v>7524</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>8351</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <v>Susie</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Susie</v>
+      </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>44532</v>
+        <v>43923</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24">
-        <v>6017</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>9715</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <v>Susie</v>
+      </c>
+      <c r="G24" t="str">
+        <v>Susie</v>
+      </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1022,7 +1004,12 @@
       <c r="D25">
         <v>6967</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="str">
+        <v>Susie</v>
+      </c>
+      <c r="G25" t="str">
+        <v>Susie</v>
+      </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1038,191 +1025,99 @@
       <c r="D26">
         <v>9624</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="str">
+        <v>Susie</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Susie</v>
+      </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>44014</v>
+        <v>44441</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D27">
-        <v>7591</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>8738</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <v>Tom</v>
+      </c>
+      <c r="G27" t="str">
+        <v>Tom</v>
+      </c>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>44532</v>
+        <v>44014</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D28">
-        <v>6295</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>7591</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <v>Tom</v>
+      </c>
+      <c r="G28" t="str">
+        <v>Tom</v>
+      </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>43953</v>
+        <v>44349</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D29">
-        <v>8738</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>6295</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <v>Tom</v>
+      </c>
+      <c r="G29" t="str">
+        <v>Tom</v>
+      </c>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>43984</v>
-      </c>
-      <c r="B30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30">
-        <v>6967</v>
-      </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="1" t="str">
+        <v>Tom</v>
+      </c>
+      <c r="G30" t="str">
+        <v>Tom</v>
+      </c>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>43953</v>
-      </c>
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31">
-        <v>9624</v>
-      </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="str">
+        <v>Tom</v>
+      </c>
+      <c r="G31" t="str">
+        <v>Tom</v>
+      </c>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>43984</v>
-      </c>
-      <c r="B32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32">
-        <v>7591</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>44014</v>
-      </c>
-      <c r="B33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33">
-        <v>6295</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>44349</v>
-      </c>
-      <c r="B34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34">
-        <v>6967</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>44441</v>
-      </c>
-      <c r="B35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35">
-        <v>9624</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>44441</v>
-      </c>
-      <c r="B36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36">
-        <v>7591</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>43953</v>
-      </c>
-      <c r="B37" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37">
-        <v>6295</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>43984</v>
-      </c>
-      <c r="B38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38">
-        <v>8738</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D29">
+    <sortCondition ref="B4:B29"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>